<commit_message>
few modifs in watchErp_2stim
</commit_message>
<xml_diff>
--- a/dataAnalysisCodes/watchERP_2stim/01-preprocess-plot/watchErpDataset.xlsx
+++ b/dataAnalysisCodes/watchERP_2stim/01-preprocess-plot/watchErpDataset.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="84">
   <si>
     <t>date</t>
   </si>
@@ -233,6 +233,39 @@
   </si>
   <si>
     <t>S06</t>
+  </si>
+  <si>
+    <t>2013-07-05-anderson</t>
+  </si>
+  <si>
+    <t>S07</t>
+  </si>
+  <si>
+    <t>anderson</t>
+  </si>
+  <si>
+    <t>2013-07-05-14-56-29-run1</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-03-20-run2</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-09-42-run3</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-21-37-run4</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-36-23-run5</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-42-28-run6</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-48-04-run7</t>
+  </si>
+  <si>
+    <t>2013-07-05-15-54-43-run8</t>
   </si>
 </sst>
 </file>
@@ -589,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +633,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -1585,6 +1618,166 @@
         <v>8</v>
       </c>
     </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>76</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D51" t="s">
+        <v>73</v>
+      </c>
+      <c r="E51" t="s">
+        <v>77</v>
+      </c>
+      <c r="F51" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C52" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D52" t="s">
+        <v>73</v>
+      </c>
+      <c r="E52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F52" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D53" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" t="s">
+        <v>79</v>
+      </c>
+      <c r="F53" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D54" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" t="s">
+        <v>80</v>
+      </c>
+      <c r="F54" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D55" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" t="s">
+        <v>81</v>
+      </c>
+      <c r="F55" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D56" t="s">
+        <v>73</v>
+      </c>
+      <c r="E56" t="s">
+        <v>82</v>
+      </c>
+      <c r="F56" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="4">
+        <v>41401</v>
+      </c>
+      <c r="D57" t="s">
+        <v>73</v>
+      </c>
+      <c r="E57" t="s">
+        <v>83</v>
+      </c>
+      <c r="F57" s="2">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>